<commit_message>
Update NBA opening night with new rosters
</commit_message>
<xml_diff>
--- a/NBA 2019-20 Opening Night/2019-10-23 - Los Angeles Lakers (102) at LA Clippers (112).xlsx
+++ b/NBA 2019-20 Opening Night/2019-10-23 - Los Angeles Lakers (102) at LA Clippers (112).xlsx
@@ -6247,7 +6247,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7864,7 +7864,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -8694,7 +8694,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -8785,7 +8785,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -8876,7 +8876,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -9240,7 +9240,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -9859,7 +9859,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -11226,7 +11226,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -11317,7 +11317,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -11754,7 +11754,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -12027,7 +12027,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -12234,7 +12234,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -12394,7 +12394,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -12940,7 +12940,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -13759,7 +13759,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -14305,7 +14305,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -14534,7 +14534,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -14625,7 +14625,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -14807,7 +14807,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -15171,7 +15171,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -15253,7 +15253,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -16465,7 +16465,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -16647,7 +16647,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -16945,7 +16945,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -17014,7 +17014,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -17381,7 +17381,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -17541,7 +17541,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -17792,7 +17792,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -17883,7 +17883,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -18831,7 +18831,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -19923,7 +19923,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -20883,7 +20883,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -21247,7 +21247,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -22121,7 +22121,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -22363,7 +22363,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -29758,7 +29758,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -31108,7 +31108,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -31381,7 +31381,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -31654,7 +31654,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -32840,7 +32840,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -33242,7 +33242,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -33515,7 +33515,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -33879,7 +33879,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -34061,7 +34061,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -34152,7 +34152,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -34883,7 +34883,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -34974,7 +34974,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -35065,7 +35065,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -35156,7 +35156,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -35329,7 +35329,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -36512,7 +36512,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -36603,7 +36603,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -36694,7 +36694,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -36785,7 +36785,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -36876,7 +36876,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -36967,7 +36967,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -37473,7 +37473,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -37542,7 +37542,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -37997,7 +37997,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -38179,7 +38179,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -38270,7 +38270,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -38807,7 +38807,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -39162,7 +39162,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -39633,7 +39633,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>DWIGHT HOWARD - #21</t>
+          <t>DWIGHT HOWARD - #39</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -41269,7 +41269,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -42342,7 +42342,7 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
@@ -42593,7 +42593,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
@@ -42775,7 +42775,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -43155,7 +43155,7 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>QUINN COOK - #4</t>
+          <t>QUINN COOK - #2</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
@@ -43293,7 +43293,7 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>JARED DUDLEY - #6</t>
+          <t>JARED DUDLEY - #10</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
@@ -45111,7 +45111,7 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B524" t="inlineStr">
@@ -46669,7 +46669,7 @@
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>MAURICE HARKLESS - #4</t>
+          <t>MAURICE HARKLESS - #8</t>
         </is>
       </c>
       <c r="B542" t="inlineStr">

</xml_diff>